<commit_message>
Creation of boxplots with probiotics
</commit_message>
<xml_diff>
--- a/03_probiotics/01_boxplots_genetics/DATOS_boxplots_probioticos.xlsx
+++ b/03_probiotics/01_boxplots_genetics/DATOS_boxplots_probioticos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luigui/Documents/shrimp_genetics_2022/03_probiotics/01_boxplots_genetics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141EB419-7A70-E44C-BC9D-9F4BE99BE2E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8ADDB39-507D-454C-ABF4-0F5EF687F945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="1" xr2:uid="{A949C7DC-2619-8949-BA62-8E2B7B3C4FFE}"/>
   </bookViews>
@@ -1334,7 +1334,7 @@
   <dimension ref="A1:T62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46:M50"/>
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2350,6 +2350,7 @@
       <c r="F43">
         <v>-2.1615337092779385</v>
       </c>
+      <c r="G43" s="1"/>
       <c r="L43" s="4" t="s">
         <v>32</v>
       </c>

</xml_diff>